<commit_message>
Deploying to gh-pages from  @ d0730a2d53f6deb63e5e85c8ce98beab8af5d93d 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/15.7.1.2.xlsx
+++ b/en/downloads/data-excel/15.7.1.2.xlsx
@@ -468,9 +468,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
@@ -478,7 +480,7 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -490,7 +492,7 @@
       </c>
       <c r="J1" s="8"/>
     </row>
-    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -502,7 +504,7 @@
       </c>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -513,8 +515,9 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -545,8 +548,11 @@
       <c r="J4" s="5">
         <v>2019</v>
       </c>
+      <c r="K4" s="5">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -576,6 +582,9 @@
       </c>
       <c r="J5" s="7">
         <v>494</v>
+      </c>
+      <c r="K5" s="7">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>